<commit_message>
Created a new file
</commit_message>
<xml_diff>
--- a/Personal_Finances.xlsx
+++ b/Personal_Finances.xlsx
@@ -553,10 +553,10 @@
         <v>2895.126652697997</v>
       </c>
       <c r="F5">
-        <v>6256.25</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="G5">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="H5">
         <v>3000</v>
@@ -568,7 +568,7 @@
         <v>12960</v>
       </c>
       <c r="K5">
-        <v>44414.65739238213</v>
+        <v>44769.86551365722</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -686,19 +686,19 @@
         <v>27</v>
       </c>
       <c r="U8">
-        <v>6256.25</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V8">
-        <v>48125</v>
+        <v>52177.49745530105</v>
       </c>
       <c r="W8">
-        <v>26950</v>
+        <v>23560</v>
       </c>
       <c r="X8">
-        <v>75075</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y8">
-        <v>721875</v>
+        <v>707822.502544699</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -751,19 +751,19 @@
         <v>28</v>
       </c>
       <c r="U9">
-        <v>6115.885416666667</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V9">
-        <v>48125</v>
+        <v>53794.99987641539</v>
       </c>
       <c r="W9">
-        <v>25265.625</v>
+        <v>21942.49757888567</v>
       </c>
       <c r="X9">
-        <v>73390.625</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y9">
-        <v>673750</v>
+        <v>654027.5026682836</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -816,19 +816,19 @@
         <v>29</v>
       </c>
       <c r="U10">
-        <v>5975.520833333333</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V10">
-        <v>48125</v>
+        <v>55462.64487258426</v>
       </c>
       <c r="W10">
-        <v>23581.25</v>
+        <v>20274.85258271679</v>
       </c>
       <c r="X10">
-        <v>71706.25</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y10">
-        <v>625625</v>
+        <v>598564.8577956994</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -881,19 +881,19 @@
         <v>30</v>
       </c>
       <c r="U11">
-        <v>5835.15625</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V11">
-        <v>48125</v>
+        <v>57181.98686363437</v>
       </c>
       <c r="W11">
-        <v>21896.875</v>
+        <v>18555.51059166668</v>
       </c>
       <c r="X11">
-        <v>70021.875</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y11">
-        <v>577500</v>
+        <v>541382.870932065</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -946,19 +946,19 @@
         <v>31</v>
       </c>
       <c r="U12">
-        <v>5694.791666666667</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V12">
-        <v>48125</v>
+        <v>58954.62845640704</v>
       </c>
       <c r="W12">
-        <v>20212.5</v>
+        <v>16782.86899889401</v>
       </c>
       <c r="X12">
-        <v>68337.5</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y12">
-        <v>529375</v>
+        <v>482428.2424756579</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1011,19 +1011,19 @@
         <v>32</v>
       </c>
       <c r="U13">
-        <v>5554.427083333333</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V13">
-        <v>48125</v>
+        <v>60782.22193855566</v>
       </c>
       <c r="W13">
-        <v>18528.125</v>
+        <v>14955.27551674539</v>
       </c>
       <c r="X13">
-        <v>66653.125</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y13">
-        <v>481250</v>
+        <v>421646.0205371022</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1076,19 +1076,19 @@
         <v>33</v>
       </c>
       <c r="U14">
-        <v>5414.0625</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V14">
-        <v>48125</v>
+        <v>62666.47081865089</v>
       </c>
       <c r="W14">
-        <v>16843.75</v>
+        <v>13071.02663665017</v>
       </c>
       <c r="X14">
-        <v>64968.75</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y14">
-        <v>433125</v>
+        <v>358979.5497184513</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -1141,19 +1141,19 @@
         <v>34</v>
       </c>
       <c r="U15">
-        <v>5273.697916666667</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V15">
-        <v>48125</v>
+        <v>64609.13141402906</v>
       </c>
       <c r="W15">
-        <v>15159.375</v>
+        <v>11128.36604127199</v>
       </c>
       <c r="X15">
-        <v>63284.375</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y15">
-        <v>385000</v>
+        <v>294370.4183044223</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -1206,19 +1206,19 @@
         <v>35</v>
       </c>
       <c r="U16">
-        <v>5133.333333333333</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V16">
-        <v>48125</v>
+        <v>66612.01448786397</v>
       </c>
       <c r="W16">
-        <v>13475</v>
+        <v>9125.48296743709</v>
       </c>
       <c r="X16">
-        <v>61600</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y16">
-        <v>336875</v>
+        <v>227758.4038165583</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -1271,19 +1271,19 @@
         <v>36</v>
       </c>
       <c r="U17">
-        <v>4992.96875</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V17">
-        <v>48125</v>
+        <v>68676.98693698774</v>
       </c>
       <c r="W17">
-        <v>11790.625</v>
+        <v>7060.510518313307</v>
       </c>
       <c r="X17">
-        <v>59915.625</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y17">
-        <v>288750</v>
+        <v>159081.4168795706</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -1336,19 +1336,19 @@
         <v>37</v>
       </c>
       <c r="U18">
-        <v>4852.604166666667</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V18">
-        <v>48125</v>
+        <v>70805.97353203436</v>
       </c>
       <c r="W18">
-        <v>10106.25</v>
+        <v>4931.523923266688</v>
       </c>
       <c r="X18">
-        <v>58231.25</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y18">
-        <v>240625</v>
+        <v>88275.44334753622</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -1401,19 +1401,19 @@
         <v>38</v>
       </c>
       <c r="U19">
-        <v>4712.239583333333</v>
+        <v>6311.458121275088</v>
       </c>
       <c r="V19">
-        <v>48125</v>
+        <v>73000.95871152743</v>
       </c>
       <c r="W19">
-        <v>8421.875</v>
+        <v>2736.538743773623</v>
       </c>
       <c r="X19">
-        <v>56546.875</v>
+        <v>75737.49745530105</v>
       </c>
       <c r="Y19">
-        <v>192500</v>
+        <v>15274.48463600878</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -1459,26 +1459,17 @@
       <c r="P20">
         <v>220163.9091882167</v>
       </c>
-      <c r="S20" s="1">
-        <v>2035</v>
-      </c>
-      <c r="T20">
-        <v>39</v>
-      </c>
-      <c r="U20">
-        <v>4571.875</v>
+      <c r="S20" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="V20">
-        <v>48125</v>
+        <v>744725.5153639911</v>
       </c>
       <c r="W20">
-        <v>6737.500000000001</v>
+        <v>164124.4540996214</v>
       </c>
       <c r="X20">
-        <v>54862.5</v>
-      </c>
-      <c r="Y20">
-        <v>144375</v>
+        <v>908849.9694636124</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -1524,27 +1515,6 @@
       <c r="P21">
         <v>195990.2569968752</v>
       </c>
-      <c r="S21" s="1">
-        <v>2036</v>
-      </c>
-      <c r="T21">
-        <v>40</v>
-      </c>
-      <c r="U21">
-        <v>4431.510416666667</v>
-      </c>
-      <c r="V21">
-        <v>48125</v>
-      </c>
-      <c r="W21">
-        <v>5053.125000000001</v>
-      </c>
-      <c r="X21">
-        <v>53178.125</v>
-      </c>
-      <c r="Y21">
-        <v>96250</v>
-      </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="1">
@@ -1589,27 +1559,6 @@
       <c r="P22">
         <v>170656.2695003492</v>
       </c>
-      <c r="S22" s="1">
-        <v>2037</v>
-      </c>
-      <c r="T22">
-        <v>41</v>
-      </c>
-      <c r="U22">
-        <v>4291.145833333333</v>
-      </c>
-      <c r="V22">
-        <v>48125</v>
-      </c>
-      <c r="W22">
-        <v>3368.75</v>
-      </c>
-      <c r="X22">
-        <v>51493.75</v>
-      </c>
-      <c r="Y22">
-        <v>48125</v>
-      </c>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="1">
@@ -1654,27 +1603,6 @@
       <c r="P23">
         <v>144106.25060399</v>
       </c>
-      <c r="S23" s="1">
-        <v>2038</v>
-      </c>
-      <c r="T23">
-        <v>42</v>
-      </c>
-      <c r="U23">
-        <v>4150.78125</v>
-      </c>
-      <c r="V23">
-        <v>48125</v>
-      </c>
-      <c r="W23">
-        <v>1684.375</v>
-      </c>
-      <c r="X23">
-        <v>49809.375</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="1">
@@ -1718,18 +1646,6 @@
       </c>
       <c r="P24">
         <v>116281.8308006056</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V24">
-        <v>770000</v>
-      </c>
-      <c r="W24">
-        <v>229075</v>
-      </c>
-      <c r="X24">
-        <v>999075</v>
       </c>
     </row>
     <row r="25" spans="1:25">

</xml_diff>